<commit_message>
adjustment import using product id
</commit_message>
<xml_diff>
--- a/public/uploads/media/default/sample_adjustments.xlsx
+++ b/public/uploads/media/default/sample_adjustments.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sahaf\Desktop\Mohamed\Sahafintech\ekstrabooks\public\uploads\media\default\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sahaf\Desktop\Mohamed\Sahafintech\ekstrabooks-v2.0\public\uploads\media\default\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2960153-CE7F-4AC0-BFC9-23BB8D3A1561}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B86DCB6-93D7-4334-BF14-750D399AD8E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{3D70032A-A14A-4146-81AC-7DD5D2E1BEA5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{3D70032A-A14A-4146-81AC-7DD5D2E1BEA5}"/>
   </bookViews>
   <sheets>
     <sheet name="sample_adjustments" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>adjustment_date</t>
   </si>
@@ -63,6 +63,9 @@
   </si>
   <si>
     <t>Materials Purchased (Frames, Lenses, Boxes, etc.)</t>
+  </si>
+  <si>
+    <t>id</t>
   </si>
 </sst>
 </file>
@@ -104,10 +107,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -442,59 +447,65 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8582DF61-F897-4B3E-8020-C8FC0D08B8D3}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.08984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.90625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="42.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.26953125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="45.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>45708</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="3">
+        <v>1827</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="1">
+      <c r="E2" s="1">
         <v>9</v>
       </c>
-      <c r="E2" s="1">
+      <c r="F2" s="1">
         <v>27</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>